<commit_message>
Gott gantt chart displaying. Everything works.
</commit_message>
<xml_diff>
--- a/web/ganttdata.xlsx
+++ b/web/ganttdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.l.spoon\web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.l.spoon\figdemo\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Task ID</t>
   </si>
@@ -65,20 +65,29 @@
     <t>Hand in paper</t>
   </si>
   <si>
-    <t>Cite, Write</t>
-  </si>
-  <si>
     <t>Outline</t>
   </si>
   <si>
     <t>Outline paper</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>Write Paper</t>
+  </si>
+  <si>
+    <t>Cite,Write</t>
+  </si>
+  <si>
+    <t>Research,Outline</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,13 +95,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF37474F"/>
+      <name val="Roboto Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7F7F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,9 +128,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,13 +418,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="42.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
@@ -404,10 +432,10 @@
     <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +458,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -447,64 +475,133 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="C3" s="1">
+        <v>42010</v>
       </c>
       <c r="D3" s="1">
-        <v>42011</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+        <v>42013</v>
       </c>
       <c r="F3">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>42010</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42011</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C5" s="1">
+        <v>42013</v>
+      </c>
+      <c r="D5" s="1">
         <v>42014</v>
       </c>
-      <c r="E4">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>42009</v>
+      </c>
+      <c r="D6" s="1">
+        <v>42010</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="4"/>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="4"/>
+      <c r="E15">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1">
-        <v>42010</v>
-      </c>
-      <c r="E5">
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="4"/>
+      <c r="E16">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4"/>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>